<commit_message>
Creacion de articulo y home
</commit_message>
<xml_diff>
--- a/Proyecto Base de datos y Diseño Web.xlsx
+++ b/Proyecto Base de datos y Diseño Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoBDDW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89105FA7-A2C8-4ACC-90DE-9DFF9F971D4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7421B538-643E-445F-B7DF-6567A937DD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
   </bookViews>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF35309-1B89-4DB1-870F-3E0240BA94B3}">
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,17 +665,17 @@
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creacion de articulos y Home con articulos
</commit_message>
<xml_diff>
--- a/Proyecto Base de datos y Diseño Web.xlsx
+++ b/Proyecto Base de datos y Diseño Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoBDDW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7421B538-643E-445F-B7DF-6567A937DD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188737F0-DFEB-4582-BB57-967F044FC3DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
   </bookViews>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF35309-1B89-4DB1-870F-3E0240BA94B3}">
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -753,7 +753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF50EE5-E637-4424-B9A1-4D4D48426474}">
   <dimension ref="B3:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30:B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correcciones de creacion de articulo
</commit_message>
<xml_diff>
--- a/Proyecto Base de datos y Diseño Web.xlsx
+++ b/Proyecto Base de datos y Diseño Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoBDDW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5690483D-B93E-41F5-90F5-E08B0515BA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712F9B8A-8D82-4807-A489-3D392F779FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
   </bookViews>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF35309-1B89-4DB1-870F-3E0240BA94B3}">
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Parte del login para perfil de usuario
</commit_message>
<xml_diff>
--- a/Proyecto Base de datos y Diseño Web.xlsx
+++ b/Proyecto Base de datos y Diseño Web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{806B3C26-D735-4679-86B3-6110A4C2CB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036F69FD-515C-4364-90F7-7FCDF091AC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
   </bookViews>
   <sheets>
     <sheet name="Fase 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Lista de actividades Proyecto Base de datos y Diseño Web</t>
   </si>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF35309-1B89-4DB1-870F-3E0240BA94B3}">
   <dimension ref="B2:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,7 +687,7 @@
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -702,14 +702,12 @@
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="B30" s="1"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
@@ -755,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF50EE5-E637-4424-B9A1-4D4D48426474}">
   <dimension ref="B3:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:B36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Terminar el home con el inicio de sesion
</commit_message>
<xml_diff>
--- a/Proyecto Base de datos y Diseño Web.xlsx
+++ b/Proyecto Base de datos y Diseño Web.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036F69FD-515C-4364-90F7-7FCDF091AC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BD0C6A-62B7-499B-AEF0-005A2549C591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
   </bookViews>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF35309-1B89-4DB1-870F-3E0240BA94B3}">
   <dimension ref="B2:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Function save article with backend correct
</commit_message>
<xml_diff>
--- a/Proyecto Base de datos y Diseño Web.xlsx
+++ b/Proyecto Base de datos y Diseño Web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBD1FAD-C952-4237-908A-16B133B92CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3A46FE-A5C2-43E1-8C5A-1ED8F314D0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
+    <workbookView xWindow="3060" yWindow="2196" windowWidth="17280" windowHeight="8880" xr2:uid="{299A2DA4-B249-45BD-B905-82C4FD62B678}"/>
   </bookViews>
   <sheets>
     <sheet name="Fase 1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Lista de actividades Proyecto Base de datos y Diseño Web</t>
   </si>
@@ -266,8 +266,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF35309-1B89-4DB1-870F-3E0240BA94B3}">
-  <dimension ref="B2:B38"/>
+  <dimension ref="B2:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,7 +612,7 @@
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -632,115 +632,120 @@
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="4" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="6" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="6" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
-        <v>44</v>
-      </c>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" s="3" t="s">
         <v>50</v>
       </c>
     </row>
@@ -753,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF50EE5-E637-4424-B9A1-4D4D48426474}">
   <dimension ref="B3:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -911,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41072B7-7C22-4B3D-B184-776107DD616A}">
   <dimension ref="B3:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>